<commit_message>
Links to the out-of-stock parts
</commit_message>
<xml_diff>
--- a/eps-eda/eps_bom/eps_BOM.xlsx
+++ b/eps-eda/eps_bom/eps_BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igeorgi1\git-repos\coloradocube\eps\eps-eda\bom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igeorgi1\git-repos\coloradocube\eps\eps-eda\eps_bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69602F0-29DB-4F72-A51E-577981F741A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F115C2AF-E314-4A5C-A73E-E984332FD48B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="259">
   <si>
     <t>FZT688BTA</t>
   </si>
@@ -815,6 +815,12 @@
   </si>
   <si>
     <t>On hand</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/maxim-integrated/MAX17055ETB-T/7200799?utm_adgroup=Analog%20Devices&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_EN_Focus%20Suppliers&amp;utm_term=&amp;utm_content=Analog%20Devices&amp;gclid=Cj0KCQjwg_iTBhDrARIsAD3Ib5iQK8v1RliAiOj7Gflk_6oZwDcZzhHUhTdLkl8Swdx256kB_BrP0YIaAsGcEALw_wcB</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/TPS61022RWUR?qs=vLWxofP3U2zlxrk4cD0iFA%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -985,15 +991,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1013,6 +1010,15 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1254,11 +1260,11 @@
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -1267,10 +1273,10 @@
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="35"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -1280,10 +1286,10 @@
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="28"/>
+      <c r="C3" s="35"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -1293,12 +1299,12 @@
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="4" t="s">
@@ -1360,10 +1366,10 @@
       <c r="E7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="30"/>
+      <c r="G7" s="40"/>
       <c r="H7" s="8" t="s">
         <v>26</v>
       </c>
@@ -1385,10 +1391,10 @@
       <c r="E8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="30"/>
+      <c r="G8" s="40"/>
       <c r="H8" s="8" t="s">
         <v>26</v>
       </c>
@@ -1409,10 +1415,10 @@
       <c r="E9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="F9" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="30"/>
+      <c r="G9" s="40"/>
       <c r="H9" s="8" t="s">
         <v>26</v>
       </c>
@@ -1433,10 +1439,10 @@
       <c r="E10" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="29" t="s">
+      <c r="F10" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="30"/>
+      <c r="G10" s="40"/>
       <c r="H10" s="8" t="s">
         <v>26</v>
       </c>
@@ -1457,10 +1463,10 @@
       <c r="E11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="29" t="s">
+      <c r="F11" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="30"/>
+      <c r="G11" s="40"/>
       <c r="H11" s="8" t="s">
         <v>26</v>
       </c>
@@ -1481,10 +1487,10 @@
       <c r="E12" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="29" t="s">
+      <c r="F12" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="30"/>
+      <c r="G12" s="40"/>
       <c r="H12" s="8" t="s">
         <v>26</v>
       </c>
@@ -1505,10 +1511,10 @@
       <c r="E13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="29" t="s">
+      <c r="F13" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="30"/>
+      <c r="G13" s="40"/>
       <c r="H13" s="8" t="s">
         <v>26</v>
       </c>
@@ -1529,10 +1535,10 @@
       <c r="E14" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="30"/>
+      <c r="G14" s="40"/>
       <c r="H14" s="8" t="s">
         <v>26</v>
       </c>
@@ -1553,10 +1559,10 @@
       <c r="E15" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="30"/>
+      <c r="G15" s="40"/>
       <c r="H15" s="8" t="s">
         <v>26</v>
       </c>
@@ -1577,10 +1583,10 @@
       <c r="E16" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="29" t="s">
+      <c r="F16" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="30"/>
+      <c r="G16" s="40"/>
       <c r="H16" s="8" t="s">
         <v>26</v>
       </c>
@@ -1601,10 +1607,10 @@
       <c r="E17" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="29" t="s">
+      <c r="F17" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="30"/>
+      <c r="G17" s="40"/>
       <c r="H17" s="8" t="s">
         <v>26</v>
       </c>
@@ -1625,10 +1631,10 @@
       <c r="E18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="27" t="s">
+      <c r="F18" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="G18" s="28"/>
+      <c r="G18" s="35"/>
       <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1">
@@ -1669,10 +1675,10 @@
       <c r="E20" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="27" t="s">
+      <c r="F20" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="G20" s="28"/>
+      <c r="G20" s="35"/>
       <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1">
@@ -1691,10 +1697,10 @@
       <c r="E21" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="27" t="s">
+      <c r="F21" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="G21" s="28"/>
+      <c r="G21" s="35"/>
       <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1">
@@ -1713,10 +1719,10 @@
       <c r="E22" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="27" t="s">
+      <c r="F22" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="G22" s="28"/>
+      <c r="G22" s="35"/>
       <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1">
@@ -1757,10 +1763,10 @@
       <c r="E24" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="27" t="s">
+      <c r="F24" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="G24" s="28"/>
+      <c r="G24" s="35"/>
       <c r="H24" s="4" t="s">
         <v>71</v>
       </c>
@@ -1781,10 +1787,10 @@
       <c r="E25" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F25" s="27" t="s">
+      <c r="F25" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="G25" s="28"/>
+      <c r="G25" s="35"/>
       <c r="H25" s="8" t="s">
         <v>55</v>
       </c>
@@ -1827,10 +1833,10 @@
       <c r="E27" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F27" s="27" t="s">
+      <c r="F27" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="G27" s="28"/>
+      <c r="G27" s="35"/>
       <c r="H27" s="8" t="s">
         <v>55</v>
       </c>
@@ -1851,10 +1857,10 @@
       <c r="E28" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F28" s="27" t="s">
+      <c r="F28" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="G28" s="28"/>
+      <c r="G28" s="35"/>
       <c r="H28" s="8" t="s">
         <v>55</v>
       </c>
@@ -1875,10 +1881,10 @@
       <c r="E29" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F29" s="27" t="s">
+      <c r="F29" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="G29" s="28"/>
+      <c r="G29" s="35"/>
       <c r="H29" s="4" t="s">
         <v>71</v>
       </c>
@@ -1899,10 +1905,10 @@
       <c r="E30" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F30" s="27" t="s">
+      <c r="F30" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="G30" s="28"/>
+      <c r="G30" s="35"/>
       <c r="H30" s="8" t="s">
         <v>55</v>
       </c>
@@ -1945,10 +1951,10 @@
       <c r="E32" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F32" s="27" t="s">
+      <c r="F32" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="G32" s="28"/>
+      <c r="G32" s="35"/>
       <c r="H32" s="8" t="s">
         <v>104</v>
       </c>
@@ -1991,10 +1997,10 @@
       <c r="E34" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F34" s="31" t="s">
+      <c r="F34" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G34" s="32"/>
+      <c r="G34" s="37"/>
       <c r="H34" s="8" t="s">
         <v>26</v>
       </c>
@@ -2015,10 +2021,10 @@
       <c r="E35" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="F35" s="31" t="s">
+      <c r="F35" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G35" s="32"/>
+      <c r="G35" s="37"/>
       <c r="H35" s="8" t="s">
         <v>26</v>
       </c>
@@ -2039,10 +2045,10 @@
       <c r="E36" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="F36" s="31" t="s">
+      <c r="F36" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G36" s="32"/>
+      <c r="G36" s="37"/>
       <c r="H36" s="8" t="s">
         <v>26</v>
       </c>
@@ -2063,10 +2069,10 @@
       <c r="E37" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="F37" s="31" t="s">
+      <c r="F37" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G37" s="32"/>
+      <c r="G37" s="37"/>
       <c r="H37" s="8" t="s">
         <v>26</v>
       </c>
@@ -2087,10 +2093,10 @@
       <c r="E38" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="F38" s="33" t="s">
+      <c r="F38" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="G38" s="32"/>
+      <c r="G38" s="37"/>
       <c r="H38" s="9"/>
     </row>
     <row r="39" spans="1:10">
@@ -2205,10 +2211,10 @@
       <c r="E43" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F43" s="31" t="s">
+      <c r="F43" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G43" s="32"/>
+      <c r="G43" s="37"/>
       <c r="H43" s="8" t="s">
         <v>26</v>
       </c>
@@ -2230,10 +2236,10 @@
       <c r="E44" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F44" s="31" t="s">
+      <c r="F44" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G44" s="32"/>
+      <c r="G44" s="37"/>
       <c r="H44" s="8" t="s">
         <v>55</v>
       </c>
@@ -2254,10 +2260,10 @@
       <c r="E45" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F45" s="31" t="s">
+      <c r="F45" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G45" s="32"/>
+      <c r="G45" s="37"/>
       <c r="H45" s="8" t="s">
         <v>26</v>
       </c>
@@ -2279,10 +2285,10 @@
       <c r="E46" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F46" s="31" t="s">
+      <c r="F46" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G46" s="32"/>
+      <c r="G46" s="37"/>
       <c r="H46" s="8" t="s">
         <v>55</v>
       </c>
@@ -2303,10 +2309,10 @@
       <c r="E47" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F47" s="31" t="s">
+      <c r="F47" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G47" s="32"/>
+      <c r="G47" s="37"/>
       <c r="H47" s="8" t="s">
         <v>26</v>
       </c>
@@ -2327,10 +2333,10 @@
       <c r="E48" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F48" s="31" t="s">
+      <c r="F48" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G48" s="32"/>
+      <c r="G48" s="37"/>
       <c r="H48" s="8" t="s">
         <v>26</v>
       </c>
@@ -2351,10 +2357,10 @@
       <c r="E49" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F49" s="27" t="s">
+      <c r="F49" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="G49" s="28"/>
+      <c r="G49" s="35"/>
       <c r="H49" s="8" t="s">
         <v>55</v>
       </c>
@@ -2397,10 +2403,10 @@
       <c r="E51" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F51" s="27" t="s">
+      <c r="F51" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="G51" s="28"/>
+      <c r="G51" s="35"/>
       <c r="H51" s="8" t="s">
         <v>26</v>
       </c>
@@ -2495,6 +2501,36 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F48:G48"/>
     <mergeCell ref="F49:G49"/>
     <mergeCell ref="F51:G51"/>
     <mergeCell ref="F36:G36"/>
@@ -2504,36 +2540,6 @@
     <mergeCell ref="F44:G44"/>
     <mergeCell ref="F45:G45"/>
     <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F7:G7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
@@ -2575,11 +2581,11 @@
       <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
@@ -2588,10 +2594,10 @@
       <c r="A2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="35"/>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
@@ -2601,10 +2607,10 @@
       <c r="A3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="28"/>
+      <c r="C3" s="35"/>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
@@ -2614,12 +2620,12 @@
       <c r="A4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
       <c r="H4" s="4" t="s">
@@ -2693,10 +2699,10 @@
       <c r="E7" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="30"/>
+      <c r="G7" s="40"/>
       <c r="H7" s="9" t="s">
         <v>26</v>
       </c>
@@ -2729,10 +2735,10 @@
       <c r="E8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="30"/>
+      <c r="G8" s="40"/>
       <c r="H8" s="9" t="s">
         <v>26</v>
       </c>
@@ -2765,10 +2771,10 @@
       <c r="E9" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="F9" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="30"/>
+      <c r="G9" s="40"/>
       <c r="H9" s="9" t="s">
         <v>26</v>
       </c>
@@ -2801,10 +2807,10 @@
       <c r="E10" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="29" t="s">
+      <c r="F10" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="30"/>
+      <c r="G10" s="40"/>
       <c r="H10" s="9" t="s">
         <v>26</v>
       </c>
@@ -2837,10 +2843,10 @@
       <c r="E11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="29" t="s">
+      <c r="F11" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="30"/>
+      <c r="G11" s="40"/>
       <c r="H11" s="9" t="s">
         <v>26</v>
       </c>
@@ -2873,10 +2879,10 @@
       <c r="E12" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="29" t="s">
+      <c r="F12" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="30"/>
+      <c r="G12" s="40"/>
       <c r="H12" s="9" t="s">
         <v>26</v>
       </c>
@@ -2909,10 +2915,10 @@
       <c r="E13" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="29" t="s">
+      <c r="F13" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="30"/>
+      <c r="G13" s="40"/>
       <c r="H13" s="9" t="s">
         <v>26</v>
       </c>
@@ -2945,10 +2951,10 @@
       <c r="E14" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="30"/>
+      <c r="G14" s="40"/>
       <c r="H14" s="9" t="s">
         <v>26</v>
       </c>
@@ -2981,10 +2987,10 @@
       <c r="E15" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="30"/>
+      <c r="G15" s="40"/>
       <c r="H15" s="9" t="s">
         <v>26</v>
       </c>
@@ -3017,10 +3023,10 @@
       <c r="E16" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="29" t="s">
+      <c r="F16" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="30"/>
+      <c r="G16" s="40"/>
       <c r="H16" s="9" t="s">
         <v>26</v>
       </c>
@@ -3053,10 +3059,10 @@
       <c r="E17" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="29" t="s">
+      <c r="F17" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="30"/>
+      <c r="G17" s="40"/>
       <c r="H17" s="9" t="s">
         <v>26</v>
       </c>
@@ -3089,10 +3095,10 @@
       <c r="E18" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="27" t="s">
+      <c r="F18" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="G18" s="28"/>
+      <c r="G18" s="35"/>
       <c r="H18" s="9"/>
       <c r="I18" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3157,10 +3163,10 @@
       <c r="E20" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="27" t="s">
+      <c r="F20" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="G20" s="28"/>
+      <c r="G20" s="35"/>
       <c r="H20" s="9"/>
       <c r="I20" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3191,10 +3197,10 @@
       <c r="E21" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="27" t="s">
+      <c r="F21" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="G21" s="28"/>
+      <c r="G21" s="35"/>
       <c r="H21" s="9"/>
       <c r="I21" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3225,10 +3231,10 @@
       <c r="E22" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="27" t="s">
+      <c r="F22" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="G22" s="28"/>
+      <c r="G22" s="35"/>
       <c r="H22" s="9"/>
       <c r="I22" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3293,10 +3299,10 @@
       <c r="E24" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="34" t="s">
+      <c r="F24" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="G24" s="35"/>
+      <c r="G24" s="42"/>
       <c r="H24" s="4" t="s">
         <v>71</v>
       </c>
@@ -3329,10 +3335,10 @@
       <c r="E25" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="F25" s="27" t="s">
+      <c r="F25" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="G25" s="28"/>
+      <c r="G25" s="35"/>
       <c r="H25" s="9" t="s">
         <v>55</v>
       </c>
@@ -3399,10 +3405,10 @@
       <c r="E27" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="F27" s="27" t="s">
+      <c r="F27" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="G27" s="28"/>
+      <c r="G27" s="35"/>
       <c r="H27" s="9" t="s">
         <v>55</v>
       </c>
@@ -3435,10 +3441,10 @@
       <c r="E28" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="F28" s="27" t="s">
+      <c r="F28" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="G28" s="28"/>
+      <c r="G28" s="35"/>
       <c r="H28" s="9" t="s">
         <v>55</v>
       </c>
@@ -3471,10 +3477,10 @@
       <c r="E29" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="F29" s="34" t="s">
+      <c r="F29" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="G29" s="35"/>
+      <c r="G29" s="42"/>
       <c r="H29" s="4" t="s">
         <v>71</v>
       </c>
@@ -3507,10 +3513,10 @@
       <c r="E30" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="F30" s="27" t="s">
+      <c r="F30" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="G30" s="28"/>
+      <c r="G30" s="35"/>
       <c r="H30" s="9" t="s">
         <v>55</v>
       </c>
@@ -3577,10 +3583,10 @@
       <c r="E32" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="F32" s="27" t="s">
+      <c r="F32" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="G32" s="28"/>
+      <c r="G32" s="35"/>
       <c r="H32" s="9" t="s">
         <v>104</v>
       </c>
@@ -3647,10 +3653,10 @@
       <c r="E34" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="F34" s="31" t="s">
+      <c r="F34" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G34" s="32"/>
+      <c r="G34" s="37"/>
       <c r="H34" s="9" t="s">
         <v>26</v>
       </c>
@@ -3683,10 +3689,10 @@
       <c r="E35" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F35" s="31" t="s">
+      <c r="F35" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G35" s="32"/>
+      <c r="G35" s="37"/>
       <c r="H35" s="9" t="s">
         <v>26</v>
       </c>
@@ -3719,10 +3725,10 @@
       <c r="E36" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F36" s="31" t="s">
+      <c r="F36" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G36" s="32"/>
+      <c r="G36" s="37"/>
       <c r="H36" s="9" t="s">
         <v>26</v>
       </c>
@@ -3755,10 +3761,10 @@
       <c r="E37" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F37" s="31" t="s">
+      <c r="F37" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G37" s="32"/>
+      <c r="G37" s="37"/>
       <c r="H37" s="9" t="s">
         <v>26</v>
       </c>
@@ -3791,10 +3797,10 @@
       <c r="E38" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="F38" s="33" t="s">
+      <c r="F38" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="G38" s="32"/>
+      <c r="G38" s="37"/>
       <c r="H38" s="9"/>
       <c r="I38" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3969,10 +3975,10 @@
       <c r="E43" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="F43" s="31" t="s">
+      <c r="F43" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G43" s="32"/>
+      <c r="G43" s="37"/>
       <c r="H43" s="9" t="s">
         <v>26</v>
       </c>
@@ -4005,10 +4011,10 @@
       <c r="E44" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="F44" s="31" t="s">
+      <c r="F44" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G44" s="32"/>
+      <c r="G44" s="37"/>
       <c r="H44" s="9" t="s">
         <v>55</v>
       </c>
@@ -4041,10 +4047,10 @@
       <c r="E45" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="F45" s="31" t="s">
+      <c r="F45" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G45" s="32"/>
+      <c r="G45" s="37"/>
       <c r="H45" s="9" t="s">
         <v>26</v>
       </c>
@@ -4077,10 +4083,10 @@
       <c r="E46" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="F46" s="31" t="s">
+      <c r="F46" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G46" s="32"/>
+      <c r="G46" s="37"/>
       <c r="H46" s="9" t="s">
         <v>55</v>
       </c>
@@ -4113,10 +4119,10 @@
       <c r="E47" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="F47" s="31" t="s">
+      <c r="F47" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G47" s="32"/>
+      <c r="G47" s="37"/>
       <c r="H47" s="9" t="s">
         <v>26</v>
       </c>
@@ -4149,10 +4155,10 @@
       <c r="E48" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="F48" s="31" t="s">
+      <c r="F48" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G48" s="32"/>
+      <c r="G48" s="37"/>
       <c r="H48" s="9" t="s">
         <v>26</v>
       </c>
@@ -4185,10 +4191,10 @@
       <c r="E49" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="F49" s="27" t="s">
+      <c r="F49" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="G49" s="28"/>
+      <c r="G49" s="35"/>
       <c r="H49" s="9" t="s">
         <v>55</v>
       </c>
@@ -4255,10 +4261,10 @@
       <c r="E51" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="F51" s="27" t="s">
+      <c r="F51" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="G51" s="28"/>
+      <c r="G51" s="35"/>
       <c r="H51" s="9" t="s">
         <v>26</v>
       </c>
@@ -4413,12 +4419,27 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="F10:G10"/>
@@ -4431,27 +4452,12 @@
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F7:G7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I4" r:id="rId1" xr:uid="{D22F4FAC-2965-4E91-A8A8-135A80C3C4BD}"/>
@@ -4466,7 +4472,7 @@
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4497,155 +4503,155 @@
       <c r="F1" s="26"/>
     </row>
     <row r="2" spans="1:7" ht="63.75">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="29" t="s">
         <v>211</v>
       </c>
-      <c r="E2" s="36"/>
+      <c r="E2" s="27"/>
     </row>
     <row r="3" spans="1:7" ht="14.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="27" t="s">
         <v>166</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="29" t="s">
         <v>212</v>
       </c>
-      <c r="E3" s="36"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="1:7" ht="25.5">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="29" t="s">
         <v>213</v>
       </c>
-      <c r="E4" s="36"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:7" ht="14.25">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="27" t="s">
         <v>166</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="D5" s="29" t="s">
         <v>212</v>
       </c>
-      <c r="E5" s="36"/>
+      <c r="E5" s="27"/>
     </row>
     <row r="6" spans="1:7" ht="25.5">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="29" t="s">
         <v>214</v>
       </c>
-      <c r="E6" s="36"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:7" ht="51">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="D7" s="29" t="s">
         <v>215</v>
       </c>
-      <c r="E7" s="36"/>
+      <c r="E7" s="27"/>
     </row>
     <row r="8" spans="1:7" ht="14.25">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="27" t="s">
         <v>170</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="29" t="s">
         <v>216</v>
       </c>
-      <c r="E8" s="36"/>
+      <c r="E8" s="27"/>
     </row>
     <row r="9" spans="1:7" ht="14.25">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="D9" s="29" t="s">
         <v>215</v>
       </c>
-      <c r="E9" s="36"/>
+      <c r="E9" s="27"/>
     </row>
     <row r="10" spans="1:7" ht="14.25">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="29" t="s">
         <v>217</v>
       </c>
-      <c r="E10" s="36"/>
+      <c r="E10" s="27"/>
     </row>
     <row r="11" spans="1:7" ht="38.25">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38" t="s">
+      <c r="D11" s="29"/>
+      <c r="E11" s="29" t="s">
         <v>218</v>
       </c>
-      <c r="F11" s="36" t="s">
+      <c r="F11" s="27" t="s">
         <v>224</v>
       </c>
       <c r="G11" t="s">
@@ -4653,20 +4659,20 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="38.25">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38" t="s">
+      <c r="D12" s="29"/>
+      <c r="E12" s="29" t="s">
         <v>218</v>
       </c>
-      <c r="F12" s="36" t="s">
+      <c r="F12" s="27" t="s">
         <v>224</v>
       </c>
       <c r="G12" t="s">
@@ -4674,35 +4680,35 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.25">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="E13" s="39"/>
+      <c r="E13" s="30"/>
     </row>
     <row r="14" spans="1:7" ht="14.25">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="36" t="s">
+      <c r="D14" s="30"/>
+      <c r="E14" s="27" t="s">
         <v>218</v>
       </c>
-      <c r="F14" s="36" t="s">
+      <c r="F14" s="27" t="s">
         <v>220</v>
       </c>
       <c r="G14" t="s">
@@ -4710,65 +4716,65 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="25.5">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="D15" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="E15" s="36"/>
+      <c r="E15" s="27"/>
     </row>
     <row r="16" spans="1:7" ht="25.5">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="38" t="s">
+      <c r="D16" s="29" t="s">
         <v>222</v>
       </c>
-      <c r="E16" s="36"/>
+      <c r="E16" s="27"/>
     </row>
     <row r="17" spans="1:7" ht="25.5">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="38" t="s">
+      <c r="D17" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="E17" s="36"/>
+      <c r="E17" s="27"/>
     </row>
     <row r="18" spans="1:7" ht="14.25">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="C18" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="39"/>
-      <c r="E18" s="37" t="s">
+      <c r="D18" s="30"/>
+      <c r="E18" s="28" t="s">
         <v>218</v>
       </c>
-      <c r="F18" s="37" t="s">
+      <c r="F18" s="28" t="s">
         <v>224</v>
       </c>
       <c r="G18" t="s">
@@ -4776,35 +4782,35 @@
       </c>
     </row>
     <row r="19" spans="1:7" s="25" customFormat="1" ht="25.5">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="31" t="s">
         <v>180</v>
       </c>
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="40" t="s">
+      <c r="C19" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="40"/>
-      <c r="E19" s="42" t="s">
+      <c r="D19" s="31"/>
+      <c r="E19" s="33" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="25.5">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="D20" s="36"/>
-      <c r="E20" s="37" t="s">
+      <c r="D20" s="27"/>
+      <c r="E20" s="28" t="s">
         <v>218</v>
       </c>
-      <c r="F20" s="37" t="s">
+      <c r="F20" s="28" t="s">
         <v>220</v>
       </c>
       <c r="G20" t="s">
@@ -4812,35 +4818,35 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="14.25">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="28" t="s">
         <v>182</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="38" t="s">
+      <c r="D21" s="29" t="s">
         <v>227</v>
       </c>
-      <c r="E21" s="36"/>
+      <c r="E21" s="27"/>
     </row>
     <row r="22" spans="1:7" ht="51">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="27" t="s">
         <v>183</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="36" t="s">
+      <c r="C22" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="D22" s="39"/>
-      <c r="E22" s="36" t="s">
+      <c r="D22" s="30"/>
+      <c r="E22" s="27" t="s">
         <v>218</v>
       </c>
-      <c r="F22" s="36" t="s">
+      <c r="F22" s="27" t="s">
         <v>220</v>
       </c>
       <c r="G22" t="s">
@@ -4848,20 +4854,20 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="38.25">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="27" t="s">
         <v>184</v>
       </c>
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="36" t="s">
+      <c r="C23" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36" t="s">
+      <c r="D23" s="27"/>
+      <c r="E23" s="27" t="s">
         <v>218</v>
       </c>
-      <c r="F23" s="36" t="s">
+      <c r="F23" s="27" t="s">
         <v>220</v>
       </c>
       <c r="G23" t="s">
@@ -4869,35 +4875,35 @@
       </c>
     </row>
     <row r="24" spans="1:7" s="25" customFormat="1" ht="38.25">
-      <c r="A24" s="40" t="s">
+      <c r="A24" s="31" t="s">
         <v>185</v>
       </c>
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="C24" s="40" t="s">
+      <c r="C24" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="40"/>
-      <c r="E24" s="42" t="s">
+      <c r="D24" s="31"/>
+      <c r="E24" s="33" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="37" t="s">
+      <c r="A25" s="28" t="s">
         <v>186</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="C25" s="36" t="s">
+      <c r="C25" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36" t="s">
+      <c r="D25" s="27"/>
+      <c r="E25" s="27" t="s">
         <v>218</v>
       </c>
-      <c r="F25" s="36" t="s">
+      <c r="F25" s="27" t="s">
         <v>220</v>
       </c>
       <c r="G25" t="s">
@@ -4905,20 +4911,20 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="37" t="s">
+      <c r="A26" s="28" t="s">
         <v>187</v>
       </c>
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="C26" s="36" t="s">
+      <c r="C26" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="D26" s="36"/>
-      <c r="E26" s="37" t="s">
+      <c r="D26" s="27"/>
+      <c r="E26" s="28" t="s">
         <v>218</v>
       </c>
-      <c r="F26" s="36" t="s">
+      <c r="F26" s="27" t="s">
         <v>224</v>
       </c>
       <c r="G26" t="s">
@@ -4926,22 +4932,22 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="25.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="D27" s="38" t="s">
+      <c r="D27" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="E27" s="37" t="s">
+      <c r="E27" s="28" t="s">
         <v>218</v>
       </c>
-      <c r="F27" s="36" t="s">
+      <c r="F27" s="27" t="s">
         <v>224</v>
       </c>
       <c r="G27" t="s">
@@ -4949,20 +4955,20 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="14.25">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="C28" s="36" t="s">
+      <c r="C28" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="D28" s="39"/>
-      <c r="E28" s="37" t="s">
+      <c r="D28" s="30"/>
+      <c r="E28" s="28" t="s">
         <v>218</v>
       </c>
-      <c r="F28" s="36" t="s">
+      <c r="F28" s="27" t="s">
         <v>220</v>
       </c>
       <c r="G28" t="s">
@@ -4970,174 +4976,174 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="38.25">
-      <c r="A29" s="36" t="s">
+      <c r="A29" s="27" t="s">
         <v>190</v>
       </c>
-      <c r="B29" s="36" t="s">
+      <c r="B29" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="C29" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="D29" s="38" t="s">
+      <c r="D29" s="29" t="s">
         <v>236</v>
       </c>
-      <c r="E29" s="36"/>
+      <c r="E29" s="27"/>
     </row>
     <row r="30" spans="1:7" ht="25.5">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="B30" s="36" t="s">
+      <c r="B30" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="C30" s="36" t="s">
+      <c r="C30" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="D30" s="38" t="s">
+      <c r="D30" s="29" t="s">
         <v>237</v>
       </c>
-      <c r="E30" s="36"/>
+      <c r="E30" s="27"/>
     </row>
     <row r="31" spans="1:7" ht="14.25">
-      <c r="A31" s="36" t="s">
+      <c r="A31" s="27" t="s">
         <v>192</v>
       </c>
-      <c r="B31" s="36" t="s">
+      <c r="B31" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="C31" s="36" t="s">
+      <c r="C31" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="D31" s="38" t="s">
+      <c r="D31" s="29" t="s">
         <v>238</v>
       </c>
-      <c r="E31" s="36"/>
+      <c r="E31" s="27"/>
     </row>
     <row r="32" spans="1:7" ht="14.25">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="27" t="s">
         <v>190</v>
       </c>
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C32" s="36" t="s">
+      <c r="C32" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="D32" s="38" t="s">
+      <c r="D32" s="29" t="s">
         <v>239</v>
       </c>
-      <c r="E32" s="36"/>
+      <c r="E32" s="27"/>
     </row>
     <row r="33" spans="1:7" ht="14.25">
-      <c r="A33" s="36" t="s">
+      <c r="A33" s="27" t="s">
         <v>193</v>
       </c>
-      <c r="B33" s="36" t="s">
+      <c r="B33" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="C33" s="36" t="s">
+      <c r="C33" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="D33" s="38" t="s">
+      <c r="D33" s="29" t="s">
         <v>242</v>
       </c>
-      <c r="E33" s="37" t="s">
+      <c r="E33" s="28" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="34" spans="1:7" s="25" customFormat="1" ht="25.5">
-      <c r="A34" s="40" t="s">
+      <c r="A34" s="31" t="s">
         <v>194</v>
       </c>
-      <c r="B34" s="40" t="s">
+      <c r="B34" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="C34" s="40" t="s">
+      <c r="C34" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="D34" s="41" t="s">
+      <c r="D34" s="32" t="s">
         <v>245</v>
       </c>
-      <c r="E34" s="42" t="s">
+      <c r="E34" s="33" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="14.25">
-      <c r="A35" s="36" t="s">
+      <c r="A35" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="B35" s="36" t="s">
+      <c r="B35" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="C35" s="36" t="s">
+      <c r="C35" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="D35" s="38" t="s">
+      <c r="D35" s="29" t="s">
         <v>236</v>
       </c>
-      <c r="E35" s="36"/>
+      <c r="E35" s="27"/>
     </row>
     <row r="36" spans="1:7" ht="14.25">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="B36" s="36" t="s">
+      <c r="B36" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="C36" s="36" t="s">
+      <c r="C36" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="D36" s="38" t="s">
+      <c r="D36" s="29" t="s">
         <v>240</v>
       </c>
-      <c r="E36" s="36"/>
+      <c r="E36" s="27"/>
     </row>
     <row r="37" spans="1:7" ht="63.75">
-      <c r="A37" s="36" t="s">
+      <c r="A37" s="27" t="s">
         <v>197</v>
       </c>
-      <c r="B37" s="36" t="s">
+      <c r="B37" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="C37" s="36" t="s">
+      <c r="C37" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="D37" s="38" t="s">
+      <c r="D37" s="29" t="s">
         <v>241</v>
       </c>
-      <c r="E37" s="36"/>
+      <c r="E37" s="27"/>
     </row>
     <row r="38" spans="1:7" ht="14.25">
-      <c r="A38" s="36" t="s">
+      <c r="A38" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="B38" s="36" t="s">
+      <c r="B38" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="C38" s="36" t="s">
+      <c r="C38" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="D38" s="38" t="s">
+      <c r="D38" s="29" t="s">
         <v>244</v>
       </c>
-      <c r="E38" s="36"/>
+      <c r="E38" s="27"/>
     </row>
     <row r="39" spans="1:7" ht="14.25">
-      <c r="A39" s="36" t="s">
+      <c r="A39" s="27" t="s">
         <v>198</v>
       </c>
-      <c r="B39" s="36" t="s">
+      <c r="B39" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="C39" s="36" t="s">
+      <c r="C39" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="D39" s="39"/>
-      <c r="E39" s="36" t="s">
+      <c r="D39" s="30"/>
+      <c r="E39" s="27" t="s">
         <v>218</v>
       </c>
-      <c r="F39" s="36" t="s">
+      <c r="F39" s="27" t="s">
         <v>220</v>
       </c>
       <c r="G39" t="s">
@@ -5145,37 +5151,37 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="14.25">
-      <c r="A40" s="37" t="s">
+      <c r="A40" s="28" t="s">
         <v>199</v>
       </c>
-      <c r="B40" s="36" t="s">
+      <c r="B40" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="C40" s="36" t="s">
+      <c r="C40" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="D40" s="38" t="s">
+      <c r="D40" s="29" t="s">
         <v>247</v>
       </c>
-      <c r="E40" s="36"/>
+      <c r="E40" s="27"/>
     </row>
     <row r="41" spans="1:7" ht="14.25">
-      <c r="A41" s="37" t="s">
+      <c r="A41" s="28" t="s">
         <v>200</v>
       </c>
-      <c r="B41" s="36" t="s">
+      <c r="B41" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="C41" s="36" t="s">
+      <c r="C41" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="D41" s="38" t="s">
+      <c r="D41" s="29" t="s">
         <v>248</v>
       </c>
-      <c r="E41" s="37" t="s">
+      <c r="E41" s="28" t="s">
         <v>218</v>
       </c>
-      <c r="F41" s="37" t="s">
+      <c r="F41" s="28" t="s">
         <v>220</v>
       </c>
       <c r="G41" t="s">
@@ -5183,50 +5189,50 @@
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="37" t="s">
+      <c r="A42" s="28" t="s">
         <v>199</v>
       </c>
-      <c r="B42" s="36" t="s">
+      <c r="B42" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="C42" s="36" t="s">
+      <c r="C42" s="27" t="s">
         <v>110</v>
       </c>
       <c r="D42" t="s">
         <v>247</v>
       </c>
-      <c r="F42" s="37"/>
+      <c r="F42" s="28"/>
     </row>
     <row r="43" spans="1:7" ht="14.25">
-      <c r="A43" s="36" t="s">
+      <c r="A43" s="27" t="s">
         <v>190</v>
       </c>
-      <c r="B43" s="36" t="s">
+      <c r="B43" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="C43" s="36" t="s">
+      <c r="C43" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="D43" s="38" t="s">
+      <c r="D43" s="29" t="s">
         <v>236</v>
       </c>
-      <c r="E43" s="36"/>
+      <c r="E43" s="27"/>
     </row>
     <row r="44" spans="1:7" ht="25.5">
-      <c r="A44" s="37" t="s">
+      <c r="A44" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="B44" s="36" t="s">
+      <c r="B44" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="C44" s="36" t="s">
+      <c r="C44" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="D44" s="39"/>
-      <c r="E44" s="37" t="s">
+      <c r="D44" s="30"/>
+      <c r="E44" s="28" t="s">
         <v>218</v>
       </c>
-      <c r="F44" s="37" t="s">
+      <c r="F44" s="28" t="s">
         <v>220</v>
       </c>
       <c r="G44" t="s">
@@ -5234,50 +5240,56 @@
       </c>
     </row>
     <row r="45" spans="1:7" s="25" customFormat="1" ht="25.5">
-      <c r="A45" s="42" t="s">
+      <c r="A45" s="33" t="s">
         <v>202</v>
       </c>
-      <c r="B45" s="40" t="s">
+      <c r="B45" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="C45" s="40" t="s">
+      <c r="C45" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="D45" s="40"/>
-      <c r="E45" s="40" t="s">
+      <c r="D45" s="31"/>
+      <c r="E45" s="31" t="s">
         <v>252</v>
       </c>
+      <c r="F45" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="G45" s="25" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="38.25">
-      <c r="A46" s="37" t="s">
+      <c r="A46" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="B46" s="36" t="s">
+      <c r="B46" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="C46" s="36" t="s">
+      <c r="C46" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="D46" s="38" t="s">
+      <c r="D46" s="29" t="s">
         <v>251</v>
       </c>
-      <c r="E46" s="36"/>
+      <c r="E46" s="27"/>
     </row>
     <row r="47" spans="1:7" ht="14.25">
-      <c r="A47" s="36" t="s">
+      <c r="A47" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="B47" s="36" t="s">
+      <c r="B47" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="C47" s="36" t="s">
+      <c r="C47" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="D47" s="39"/>
-      <c r="E47" s="36" t="s">
+      <c r="D47" s="30"/>
+      <c r="E47" s="27" t="s">
         <v>218</v>
       </c>
-      <c r="F47" s="36" t="s">
+      <c r="F47" s="27" t="s">
         <v>220</v>
       </c>
       <c r="G47" t="s">
@@ -5285,49 +5297,55 @@
       </c>
     </row>
     <row r="48" spans="1:7" s="25" customFormat="1" ht="25.5">
-      <c r="A48" s="42" t="s">
+      <c r="A48" s="33" t="s">
         <v>205</v>
       </c>
-      <c r="B48" s="40" t="s">
+      <c r="B48" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="C48" s="40" t="s">
+      <c r="C48" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="D48" s="41" t="s">
+      <c r="D48" s="32" t="s">
         <v>254</v>
       </c>
-      <c r="E48" s="42" t="s">
+      <c r="E48" s="33" t="s">
         <v>252</v>
       </c>
+      <c r="F48" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="G48" s="25" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="49" spans="1:5" ht="14.25">
-      <c r="A49" s="37" t="s">
+      <c r="A49" s="28" t="s">
         <v>206</v>
       </c>
-      <c r="B49" s="36" t="s">
+      <c r="B49" s="27" t="s">
         <v>155</v>
       </c>
-      <c r="C49" s="36" t="s">
+      <c r="C49" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="D49" s="39"/>
-      <c r="E49" s="37" t="s">
+      <c r="D49" s="30"/>
+      <c r="E49" s="28" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="36" t="s">
+      <c r="A50" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="B50" s="36" t="s">
+      <c r="B50" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="C50" s="36" t="s">
+      <c r="C50" s="27" t="s">
         <v>161</v>
       </c>
-      <c r="D50" s="36"/>
-      <c r="E50" s="37" t="s">
+      <c r="D50" s="27"/>
+      <c r="E50" s="28" t="s">
         <v>256</v>
       </c>
     </row>

</xml_diff>